<commit_message>
Group by and Let function added
</commit_message>
<xml_diff>
--- a/Sum.xlsx
+++ b/Sum.xlsx
@@ -1,19 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DINESH\Ui-Path\Linq_Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dinesh Shakyawar\Pictures\Dinesh\Dinesh Personal\UiPath\Linq-Ui-Path\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E16267-934A-42CE-B2A8-F58D9069FE89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F128836-EE11-4AFE-B2E6-884331233C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2976" yWindow="2064" windowWidth="17280" windowHeight="8880" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Duplicate Only CityID" sheetId="5" r:id="rId2"/>
+    <sheet name="Unique CityID" sheetId="4" r:id="rId3"/>
+    <sheet name="Group by CityID" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="Modify Items" sheetId="7" r:id="rId6"/>
+    <sheet name="Modify Items3" sheetId="10" r:id="rId7"/>
+    <sheet name="Modify Items2" sheetId="9" r:id="rId8"/>
+    <sheet name="Modify Items1" sheetId="8" r:id="rId9"/>
+    <sheet name="Let Keyword" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="52">
   <si>
     <t>Emp Name</t>
   </si>
@@ -64,6 +73,123 @@
   </si>
   <si>
     <t>Age</t>
+  </si>
+  <si>
+    <t>CityID</t>
+  </si>
+  <si>
+    <t>CityName</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Frankfurt</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
+    <t>Ontario</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>01.01.2010</t>
+  </si>
+  <si>
+    <t>07.05.2021</t>
+  </si>
+  <si>
+    <t>04.07.2019</t>
+  </si>
+  <si>
+    <t>16.12.2015</t>
+  </si>
+  <si>
+    <t>03.10.2000</t>
+  </si>
+  <si>
+    <t>17.04.2012</t>
+  </si>
+  <si>
+    <t>30.09.2017</t>
+  </si>
+  <si>
+    <t>15.11.2018</t>
+  </si>
+  <si>
+    <t>12.10.2011</t>
+  </si>
+  <si>
+    <t>21.05.2014</t>
+  </si>
+  <si>
+    <t>19.07.2016</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Milk</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Tomato</t>
+  </si>
+  <si>
+    <t>Potato</t>
+  </si>
+  <si>
+    <t>Fish</t>
+  </si>
+  <si>
+    <t>Meat</t>
+  </si>
+  <si>
+    <t>.Milk</t>
+  </si>
+  <si>
+    <t>^2127</t>
+  </si>
+  <si>
+    <t>^1321</t>
+  </si>
+  <si>
+    <t>.Fish</t>
+  </si>
+  <si>
+    <t>Rice Neagtive</t>
   </si>
 </sst>
 </file>
@@ -383,17 +509,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,7 +536,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -427,7 +553,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -444,7 +570,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -461,7 +587,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -478,7 +604,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -493,6 +619,1069 @@
       </c>
       <c r="E6">
         <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453A4EFD-D1A5-4572-B7D6-896648FF1E51}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2">
+        <v>1.5</v>
+      </c>
+      <c r="D2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>5324</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3">
+        <v>1.6</v>
+      </c>
+      <c r="D3">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4255</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4">
+        <v>1.7</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5">
+        <v>3.5</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5352</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6333</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2681298D-9360-4EBF-B354-3C11288DB195}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>41113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5">
+        <v>846</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB75E677-E599-4C05-95BF-A8E93ED5D225}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2">
+        <v>6411</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <v>54641</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>21321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6">
+        <v>8464</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7">
+        <v>84641</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8">
+        <v>654</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D573B1-2417-497D-89DD-96526654E179}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>41113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3">
+        <v>6411</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4">
+        <v>54641</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>21321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7">
+        <v>8464</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8">
+        <v>84641</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10">
+        <v>465</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73615FF3-BB9F-4675-A515-DD8AEF5BCC67}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>41113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4">
+        <v>6411</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>54641</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>21321</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8">
+        <v>8464</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9">
+        <v>84641</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12">
+        <v>846</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2402D2DC-275D-4624-A75E-047C8B999002}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2127</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>5324</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4255</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1321</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5352</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6333</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791B9927-A9B1-46FC-8EAA-85F3E3392A5B}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2127</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>1.5</v>
+      </c>
+      <c r="D2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>4255</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3">
+        <v>1.7</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1321</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4">
+        <v>3.5</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5352</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6333</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DE1321-0789-45DA-BFA1-C832E04C2510}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>5324</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2">
+        <v>1.6</v>
+      </c>
+      <c r="D2">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2127</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3">
+        <v>1.5</v>
+      </c>
+      <c r="D3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4255</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4">
+        <v>1.7</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1321</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5">
+        <v>3.5</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5352</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6333</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D75726-BE5B-4B37-A65E-E442BD1ABDC7}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2127</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>1.5</v>
+      </c>
+      <c r="D2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>5324</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3">
+        <v>1.6</v>
+      </c>
+      <c r="D3">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4255</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4">
+        <v>1.7</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1321</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5">
+        <v>3.5</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5352</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6333</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>